<commit_message>
Segg the new transmittals and included the data files for poc
</commit_message>
<xml_diff>
--- a/Falcrum_Trunk/src/com/proj/config/Config.xlsx
+++ b/Falcrum_Trunk/src/com/proj/config/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeapThoughtProjectWS\Falcrum_Trunk\src\com\proj\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIWS\Falcrum_Trunk\src\com\proj\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>\\src\\com\\proj\\suiteDOCS\\testdata\\DocumentsTestData.xlsx</t>
+  </si>
+  <si>
+    <t>Transmittals_New_Correspondence</t>
+  </si>
+  <si>
+    <t>Transmittals_New_ConsultantAdvice</t>
+  </si>
+  <si>
+    <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\TransmittalsTestData-Correspondence.xlsx</t>
+  </si>
+  <si>
+    <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\TransmittalsTestData-ConsultantAdvice.xlsx</t>
+  </si>
+  <si>
+    <t>Transmittals_New_ChangeNote</t>
+  </si>
+  <si>
+    <t>\\src\\com\\proj\\suiteTRANSMITTALS\\testdata\\TransmittalsTestData-ChangeNote.xlsx</t>
   </si>
 </sst>
 </file>
@@ -505,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -535,15 +553,39 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6">
       <formula1>"XL,DB"</formula1>
     </dataValidation>
   </dataValidations>
@@ -555,9 +597,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -590,23 +634,59 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>